<commit_message>
Finished console excel converter
</commit_message>
<xml_diff>
--- a/PetaPolaKuman/ExcelRSMA.xlsx
+++ b/PetaPolaKuman/ExcelRSMA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobby\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobby\source\repos\PetaPolaKuman\PetaPolaKuman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD17499F-A00F-4213-A287-21E1943BA89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9974F931-C02C-4D77-AC4B-FF1E3804BF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -933,11 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AZ244"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G265" sqref="G265"/>
+      <selection activeCell="L244" sqref="L244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1112,7 +1111,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>56582</v>
       </c>
@@ -1203,7 +1202,7 @@
       <c r="AX2" s="10"/>
       <c r="AY2" s="10"/>
     </row>
-    <row r="3" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>5703</v>
       </c>
@@ -1300,7 +1299,7 @@
       </c>
       <c r="AY3" s="10"/>
     </row>
-    <row r="4" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>42371</v>
       </c>
@@ -1389,7 +1388,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>42054</v>
       </c>
@@ -1476,7 +1475,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4278</v>
       </c>
@@ -1549,7 +1548,7 @@
       </c>
       <c r="AY6" s="10"/>
     </row>
-    <row r="7" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>42826</v>
       </c>
@@ -1620,7 +1619,7 @@
       <c r="AX7" s="10"/>
       <c r="AY7" s="10"/>
     </row>
-    <row r="8" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>46250</v>
       </c>
@@ -1693,7 +1692,7 @@
       <c r="AX8" s="10"/>
       <c r="AY8" s="10"/>
     </row>
-    <row r="9" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>53950</v>
       </c>
@@ -1770,7 +1769,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>65166</v>
       </c>
@@ -1863,7 +1862,7 @@
       </c>
       <c r="AY10" s="10"/>
     </row>
-    <row r="11" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>67023</v>
       </c>
@@ -1952,7 +1951,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>84919</v>
       </c>
@@ -2045,7 +2044,7 @@
       </c>
       <c r="AY12" s="10"/>
     </row>
-    <row r="13" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1450</v>
       </c>
@@ -2130,7 +2129,7 @@
       </c>
       <c r="AY13" s="10"/>
     </row>
-    <row r="14" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>5313</v>
       </c>
@@ -2217,7 +2216,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>12534</v>
       </c>
@@ -2288,7 +2287,7 @@
       <c r="AX15" s="10"/>
       <c r="AY15" s="10"/>
     </row>
-    <row r="16" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>12149</v>
       </c>
@@ -2375,7 +2374,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>11957</v>
       </c>
@@ -2454,7 +2453,7 @@
       <c r="AX17" s="10"/>
       <c r="AY17" s="10"/>
     </row>
-    <row r="18" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>14461</v>
       </c>
@@ -2539,7 +2538,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>15059</v>
       </c>
@@ -2626,7 +2625,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>14800</v>
       </c>
@@ -2697,7 +2696,7 @@
       <c r="AX20" s="10"/>
       <c r="AY20" s="10"/>
     </row>
-    <row r="21" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>16373</v>
       </c>
@@ -2768,7 +2767,7 @@
       <c r="AX21" s="10"/>
       <c r="AY21" s="10"/>
     </row>
-    <row r="22" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>16806</v>
       </c>
@@ -2839,7 +2838,7 @@
       <c r="AX22" s="10"/>
       <c r="AY22" s="10"/>
     </row>
-    <row r="23" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>16433</v>
       </c>
@@ -2910,7 +2909,7 @@
       <c r="AX23" s="10"/>
       <c r="AY23" s="10"/>
     </row>
-    <row r="24" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>17501</v>
       </c>
@@ -2999,7 +2998,7 @@
       </c>
       <c r="AY24" s="10"/>
     </row>
-    <row r="25" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>17587</v>
       </c>
@@ -3070,7 +3069,7 @@
       <c r="AX25" s="10"/>
       <c r="AY25" s="10"/>
     </row>
-    <row r="26" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>29796</v>
       </c>
@@ -3155,7 +3154,7 @@
       </c>
       <c r="AY26" s="10"/>
     </row>
-    <row r="27" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>40090</v>
       </c>
@@ -3246,7 +3245,7 @@
       <c r="AX27" s="10"/>
       <c r="AY27" s="10"/>
     </row>
-    <row r="28" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44812</v>
       </c>
@@ -3331,7 +3330,7 @@
       </c>
       <c r="AY28" s="10"/>
     </row>
-    <row r="29" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>56568</v>
       </c>
@@ -3408,7 +3407,7 @@
       </c>
       <c r="AY29" s="10"/>
     </row>
-    <row r="30" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>59945</v>
       </c>
@@ -3495,7 +3494,7 @@
       </c>
       <c r="AY30" s="10"/>
     </row>
-    <row r="31" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>62261</v>
       </c>
@@ -3590,7 +3589,7 @@
       </c>
       <c r="AY31" s="10"/>
     </row>
-    <row r="32" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>68997</v>
       </c>
@@ -3671,7 +3670,7 @@
       </c>
       <c r="AY32" s="10"/>
     </row>
-    <row r="33" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>69143</v>
       </c>
@@ -3754,7 +3753,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>69444</v>
       </c>
@@ -3825,7 +3824,7 @@
       <c r="AX34" s="10"/>
       <c r="AY34" s="10"/>
     </row>
-    <row r="35" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>72260</v>
       </c>
@@ -3914,7 +3913,7 @@
       </c>
       <c r="AY35" s="10"/>
     </row>
-    <row r="36" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>79476</v>
       </c>
@@ -4001,7 +4000,7 @@
       </c>
       <c r="AY36" s="10"/>
     </row>
-    <row r="37" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>64622</v>
       </c>
@@ -4080,7 +4079,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>2403</v>
       </c>
@@ -4167,7 +4166,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>2402</v>
       </c>
@@ -4238,7 +4237,7 @@
       <c r="AX39" s="10"/>
       <c r="AY39" s="10"/>
     </row>
-    <row r="40" spans="1:51" ht="52.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:51" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>15772</v>
       </c>
@@ -4333,7 +4332,7 @@
       </c>
       <c r="AY40" s="10"/>
     </row>
-    <row r="41" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>20968</v>
       </c>
@@ -4430,7 +4429,7 @@
       <c r="AX41" s="10"/>
       <c r="AY41" s="10"/>
     </row>
-    <row r="42" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>21955</v>
       </c>
@@ -4531,7 +4530,7 @@
       </c>
       <c r="AY42" s="10"/>
     </row>
-    <row r="43" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>21955</v>
       </c>
@@ -4632,7 +4631,7 @@
       </c>
       <c r="AY43" s="10"/>
     </row>
-    <row r="44" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>22251</v>
       </c>
@@ -4731,7 +4730,7 @@
       </c>
       <c r="AY44" s="10"/>
     </row>
-    <row r="45" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>21945</v>
       </c>
@@ -4826,7 +4825,7 @@
       </c>
       <c r="AY45" s="10"/>
     </row>
-    <row r="46" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>24964</v>
       </c>
@@ -4925,7 +4924,7 @@
       </c>
       <c r="AY46" s="10"/>
     </row>
-    <row r="47" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>26587</v>
       </c>
@@ -5024,7 +5023,7 @@
       </c>
       <c r="AY47" s="10"/>
     </row>
-    <row r="48" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>27468</v>
       </c>
@@ -5095,7 +5094,7 @@
       <c r="AX48" s="10"/>
       <c r="AY48" s="10"/>
     </row>
-    <row r="49" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>30317</v>
       </c>
@@ -5168,7 +5167,7 @@
       <c r="AX49" s="10"/>
       <c r="AY49" s="10"/>
     </row>
-    <row r="50" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>32841</v>
       </c>
@@ -5239,7 +5238,7 @@
       <c r="AX50" s="10"/>
       <c r="AY50" s="10"/>
     </row>
-    <row r="51" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>32857</v>
       </c>
@@ -5310,7 +5309,7 @@
       <c r="AX51" s="10"/>
       <c r="AY51" s="10"/>
     </row>
-    <row r="52" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>33359</v>
       </c>
@@ -5409,7 +5408,7 @@
       </c>
       <c r="AY52" s="10"/>
     </row>
-    <row r="53" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>39712</v>
       </c>
@@ -5480,7 +5479,7 @@
       <c r="AX53" s="10"/>
       <c r="AY53" s="10"/>
     </row>
-    <row r="54" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>42083</v>
       </c>
@@ -5573,7 +5572,7 @@
       <c r="AX54" s="10"/>
       <c r="AY54" s="10"/>
     </row>
-    <row r="55" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>42083</v>
       </c>
@@ -5662,7 +5661,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>40924</v>
       </c>
@@ -5749,7 +5748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>46251</v>
       </c>
@@ -5842,7 +5841,7 @@
       </c>
       <c r="AY57" s="10"/>
     </row>
-    <row r="58" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>45704</v>
       </c>
@@ -5913,7 +5912,7 @@
       <c r="AX58" s="10"/>
       <c r="AY58" s="10"/>
     </row>
-    <row r="59" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>45155</v>
       </c>
@@ -6010,7 +6009,7 @@
       </c>
       <c r="AY59" s="10"/>
     </row>
-    <row r="60" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>45956</v>
       </c>
@@ -6099,7 +6098,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>40009</v>
       </c>
@@ -6192,7 +6191,7 @@
       </c>
       <c r="AY61" s="10"/>
     </row>
-    <row r="62" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>48248</v>
       </c>
@@ -6289,7 +6288,7 @@
       </c>
       <c r="AY62" s="10"/>
     </row>
-    <row r="63" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>50278</v>
       </c>
@@ -6380,7 +6379,7 @@
       <c r="AX63" s="10"/>
       <c r="AY63" s="10"/>
     </row>
-    <row r="64" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>56065</v>
       </c>
@@ -6471,7 +6470,7 @@
       </c>
       <c r="AY64" s="10"/>
     </row>
-    <row r="65" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>62797</v>
       </c>
@@ -6558,7 +6557,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>66127</v>
       </c>
@@ -6657,7 +6656,7 @@
       </c>
       <c r="AY66" s="10"/>
     </row>
-    <row r="67" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>68284</v>
       </c>
@@ -6752,7 +6751,7 @@
       </c>
       <c r="AY67" s="10"/>
     </row>
-    <row r="68" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>70925</v>
       </c>
@@ -6837,7 +6836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>72785</v>
       </c>
@@ -6914,7 +6913,7 @@
       <c r="AX69" s="10"/>
       <c r="AY69" s="10"/>
     </row>
-    <row r="70" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>73465</v>
       </c>
@@ -7005,7 +7004,7 @@
       </c>
       <c r="AY70" s="10"/>
     </row>
-    <row r="71" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>74507</v>
       </c>
@@ -7082,7 +7081,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>75466</v>
       </c>
@@ -7169,7 +7168,7 @@
       </c>
       <c r="AY72" s="10"/>
     </row>
-    <row r="73" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>74808</v>
       </c>
@@ -7258,7 +7257,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>77872</v>
       </c>
@@ -7357,7 +7356,7 @@
       </c>
       <c r="AY74" s="10"/>
     </row>
-    <row r="75" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>77892</v>
       </c>
@@ -7446,7 +7445,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>79469</v>
       </c>
@@ -7541,7 +7540,7 @@
       </c>
       <c r="AY76" s="10"/>
     </row>
-    <row r="77" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>80470</v>
       </c>
@@ -7632,7 +7631,7 @@
       </c>
       <c r="AY77" s="10"/>
     </row>
-    <row r="78" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>84147</v>
       </c>
@@ -7729,7 +7728,7 @@
       </c>
       <c r="AY78" s="10"/>
     </row>
-    <row r="79" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>82712</v>
       </c>
@@ -7822,7 +7821,7 @@
       </c>
       <c r="AY79" s="10"/>
     </row>
-    <row r="80" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>82681</v>
       </c>
@@ -7911,7 +7910,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>13061</v>
       </c>
@@ -7982,7 +7981,7 @@
       <c r="AX81" s="10"/>
       <c r="AY81" s="10"/>
     </row>
-    <row r="82" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>14380</v>
       </c>
@@ -8053,7 +8052,7 @@
       <c r="AX82" s="10"/>
       <c r="AY82" s="10"/>
     </row>
-    <row r="83" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>16373</v>
       </c>
@@ -8124,7 +8123,7 @@
       <c r="AX83" s="10"/>
       <c r="AY83" s="10"/>
     </row>
-    <row r="84" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>15624</v>
       </c>
@@ -8195,7 +8194,7 @@
       <c r="AX84" s="10"/>
       <c r="AY84" s="10"/>
     </row>
-    <row r="85" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>17291</v>
       </c>
@@ -8266,7 +8265,7 @@
       <c r="AX85" s="10"/>
       <c r="AY85" s="10"/>
     </row>
-    <row r="86" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>17284</v>
       </c>
@@ -8337,7 +8336,7 @@
       <c r="AX86" s="10"/>
       <c r="AY86" s="10"/>
     </row>
-    <row r="87" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>16873</v>
       </c>
@@ -8414,7 +8413,7 @@
       </c>
       <c r="AY87" s="10"/>
     </row>
-    <row r="88" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>18138</v>
       </c>
@@ -8485,7 +8484,7 @@
       <c r="AX88" s="10"/>
       <c r="AY88" s="10"/>
     </row>
-    <row r="89" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>21296</v>
       </c>
@@ -8556,7 +8555,7 @@
       <c r="AX89" s="10"/>
       <c r="AY89" s="10"/>
     </row>
-    <row r="90" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>19068</v>
       </c>
@@ -8627,7 +8626,7 @@
       <c r="AX90" s="10"/>
       <c r="AY90" s="10"/>
     </row>
-    <row r="91" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>19343</v>
       </c>
@@ -8714,7 +8713,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="92" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>22195</v>
       </c>
@@ -8803,7 +8802,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>22258</v>
       </c>
@@ -8874,7 +8873,7 @@
       <c r="AX93" s="10"/>
       <c r="AY93" s="10"/>
     </row>
-    <row r="94" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>25301</v>
       </c>
@@ -8945,7 +8944,7 @@
       <c r="AX94" s="10"/>
       <c r="AY94" s="10"/>
     </row>
-    <row r="95" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>23785</v>
       </c>
@@ -9016,7 +9015,7 @@
       <c r="AX95" s="10"/>
       <c r="AY95" s="10"/>
     </row>
-    <row r="96" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>24524</v>
       </c>
@@ -9087,7 +9086,7 @@
       <c r="AX96" s="10"/>
       <c r="AY96" s="10"/>
     </row>
-    <row r="97" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>23785</v>
       </c>
@@ -9174,7 +9173,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>27846</v>
       </c>
@@ -9251,7 +9250,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>25658</v>
       </c>
@@ -9322,7 +9321,7 @@
       <c r="AX99" s="10"/>
       <c r="AY99" s="10"/>
     </row>
-    <row r="100" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>25837</v>
       </c>
@@ -9409,7 +9408,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>26916</v>
       </c>
@@ -9480,7 +9479,7 @@
       <c r="AX101" s="10"/>
       <c r="AY101" s="10"/>
     </row>
-    <row r="102" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>26339</v>
       </c>
@@ -9551,7 +9550,7 @@
       <c r="AX102" s="10"/>
       <c r="AY102" s="10"/>
     </row>
-    <row r="103" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>25807</v>
       </c>
@@ -9622,7 +9621,7 @@
       <c r="AX103" s="10"/>
       <c r="AY103" s="10"/>
     </row>
-    <row r="104" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>25451</v>
       </c>
@@ -9711,7 +9710,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="105" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>31522</v>
       </c>
@@ -9782,7 +9781,7 @@
       <c r="AX105" s="10"/>
       <c r="AY105" s="10"/>
     </row>
-    <row r="106" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>29822</v>
       </c>
@@ -9853,7 +9852,7 @@
       <c r="AX106" s="10"/>
       <c r="AY106" s="10"/>
     </row>
-    <row r="107" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>32022</v>
       </c>
@@ -9942,7 +9941,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="108" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>32806</v>
       </c>
@@ -10013,7 +10012,7 @@
       <c r="AX108" s="10"/>
       <c r="AY108" s="10"/>
     </row>
-    <row r="109" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>31099</v>
       </c>
@@ -10084,7 +10083,7 @@
       <c r="AX109" s="10"/>
       <c r="AY109" s="10"/>
     </row>
-    <row r="110" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>33300</v>
       </c>
@@ -10155,7 +10154,7 @@
       <c r="AX110" s="10"/>
       <c r="AY110" s="10"/>
     </row>
-    <row r="111" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>33668</v>
       </c>
@@ -10226,7 +10225,7 @@
       <c r="AX111" s="10"/>
       <c r="AY111" s="10"/>
     </row>
-    <row r="112" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>33649</v>
       </c>
@@ -10297,7 +10296,7 @@
       <c r="AX112" s="10"/>
       <c r="AY112" s="10"/>
     </row>
-    <row r="113" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>35310</v>
       </c>
@@ -10368,7 +10367,7 @@
       <c r="AX113" s="10"/>
       <c r="AY113" s="10"/>
     </row>
-    <row r="114" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>35650</v>
       </c>
@@ -10457,7 +10456,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>32359</v>
       </c>
@@ -10548,7 +10547,7 @@
       <c r="AX115" s="10"/>
       <c r="AY115" s="10"/>
     </row>
-    <row r="116" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>35030</v>
       </c>
@@ -10637,7 +10636,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="117" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>31476</v>
       </c>
@@ -10708,7 +10707,7 @@
       <c r="AX117" s="10"/>
       <c r="AY117" s="10"/>
     </row>
-    <row r="118" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>12193</v>
       </c>
@@ -10779,7 +10778,7 @@
       <c r="AX118" s="10"/>
       <c r="AY118" s="10"/>
     </row>
-    <row r="119" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>10436</v>
       </c>
@@ -10856,7 +10855,7 @@
       </c>
       <c r="AY119" s="10"/>
     </row>
-    <row r="120" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>6082</v>
       </c>
@@ -10933,7 +10932,7 @@
       </c>
       <c r="AY120" s="10"/>
     </row>
-    <row r="121" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>4296</v>
       </c>
@@ -11004,7 +11003,7 @@
       <c r="AX121" s="10"/>
       <c r="AY121" s="10"/>
     </row>
-    <row r="122" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>2709</v>
       </c>
@@ -11075,7 +11074,7 @@
       <c r="AX122" s="10"/>
       <c r="AY122" s="10"/>
     </row>
-    <row r="123" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>6092</v>
       </c>
@@ -11146,7 +11145,7 @@
       <c r="AX123" s="10"/>
       <c r="AY123" s="10"/>
     </row>
-    <row r="124" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>13516</v>
       </c>
@@ -11217,7 +11216,7 @@
       <c r="AX124" s="10"/>
       <c r="AY124" s="10"/>
     </row>
-    <row r="125" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>14157</v>
       </c>
@@ -11316,7 +11315,7 @@
       </c>
       <c r="AY125" s="10"/>
     </row>
-    <row r="126" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>14149</v>
       </c>
@@ -11393,7 +11392,7 @@
       </c>
       <c r="AY126" s="10"/>
     </row>
-    <row r="127" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>14147</v>
       </c>
@@ -11464,7 +11463,7 @@
       <c r="AX127" s="10"/>
       <c r="AY127" s="10"/>
     </row>
-    <row r="128" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>14799</v>
       </c>
@@ -11535,7 +11534,7 @@
       <c r="AX128" s="10"/>
       <c r="AY128" s="10"/>
     </row>
-    <row r="129" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>35622</v>
       </c>
@@ -11606,7 +11605,7 @@
       <c r="AX129" s="10"/>
       <c r="AY129" s="10"/>
     </row>
-    <row r="130" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>37566</v>
       </c>
@@ -11677,7 +11676,7 @@
       <c r="AX130" s="10"/>
       <c r="AY130" s="10"/>
     </row>
-    <row r="131" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>39214</v>
       </c>
@@ -11748,7 +11747,7 @@
       <c r="AX131" s="10"/>
       <c r="AY131" s="10"/>
     </row>
-    <row r="132" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>40924</v>
       </c>
@@ -11819,7 +11818,7 @@
       <c r="AX132" s="10"/>
       <c r="AY132" s="10"/>
     </row>
-    <row r="133" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>39512</v>
       </c>
@@ -11890,7 +11889,7 @@
       <c r="AX133" s="10"/>
       <c r="AY133" s="10"/>
     </row>
-    <row r="134" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>45957</v>
       </c>
@@ -11979,7 +11978,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="135" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>43071</v>
       </c>
@@ -12066,7 +12065,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="136" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>42090</v>
       </c>
@@ -12137,7 +12136,7 @@
       <c r="AX136" s="10"/>
       <c r="AY136" s="10"/>
     </row>
-    <row r="137" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>46294</v>
       </c>
@@ -12212,7 +12211,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="138" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>47439</v>
       </c>
@@ -12283,7 +12282,7 @@
       <c r="AX138" s="10"/>
       <c r="AY138" s="10"/>
     </row>
-    <row r="139" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>40413</v>
       </c>
@@ -12354,7 +12353,7 @@
       <c r="AX139" s="10"/>
       <c r="AY139" s="10"/>
     </row>
-    <row r="140" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>44861</v>
       </c>
@@ -12443,7 +12442,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="141" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>47247</v>
       </c>
@@ -12530,7 +12529,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="142" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>52106</v>
       </c>
@@ -12619,7 +12618,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="143" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>50834</v>
       </c>
@@ -12690,7 +12689,7 @@
       <c r="AX143" s="10"/>
       <c r="AY143" s="10"/>
     </row>
-    <row r="144" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>51120</v>
       </c>
@@ -12761,7 +12760,7 @@
       <c r="AX144" s="10"/>
       <c r="AY144" s="10"/>
     </row>
-    <row r="145" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>49894</v>
       </c>
@@ -12838,7 +12837,7 @@
       <c r="AX145" s="10"/>
       <c r="AY145" s="10"/>
     </row>
-    <row r="146" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>52883</v>
       </c>
@@ -12925,7 +12924,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="147" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>51720</v>
       </c>
@@ -13012,7 +13011,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="148" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>52583</v>
       </c>
@@ -13101,7 +13100,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="149" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>54909</v>
       </c>
@@ -13172,7 +13171,7 @@
       <c r="AX149" s="10"/>
       <c r="AY149" s="10"/>
     </row>
-    <row r="150" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>55285</v>
       </c>
@@ -13243,7 +13242,7 @@
       <c r="AX150" s="10"/>
       <c r="AY150" s="10"/>
     </row>
-    <row r="151" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>54462</v>
       </c>
@@ -13314,7 +13313,7 @@
       <c r="AX151" s="10"/>
       <c r="AY151" s="10"/>
     </row>
-    <row r="152" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>55717</v>
       </c>
@@ -13385,7 +13384,7 @@
       <c r="AX152" s="10"/>
       <c r="AY152" s="10"/>
     </row>
-    <row r="153" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>57860</v>
       </c>
@@ -13458,7 +13457,7 @@
       <c r="AX153" s="10"/>
       <c r="AY153" s="10"/>
     </row>
-    <row r="154" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>52639</v>
       </c>
@@ -13545,7 +13544,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="155" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>58792</v>
       </c>
@@ -13616,7 +13615,7 @@
       <c r="AX155" s="10"/>
       <c r="AY155" s="10"/>
     </row>
-    <row r="156" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>58679</v>
       </c>
@@ -13687,7 +13686,7 @@
       <c r="AX156" s="10"/>
       <c r="AY156" s="10"/>
     </row>
-    <row r="157" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>52639</v>
       </c>
@@ -13758,7 +13757,7 @@
       <c r="AX157" s="10"/>
       <c r="AY157" s="10"/>
     </row>
-    <row r="158" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>57159</v>
       </c>
@@ -13829,7 +13828,7 @@
       <c r="AX158" s="10"/>
       <c r="AY158" s="10"/>
     </row>
-    <row r="159" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>60206</v>
       </c>
@@ -13900,7 +13899,7 @@
       <c r="AX159" s="10"/>
       <c r="AY159" s="10"/>
     </row>
-    <row r="160" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>47849</v>
       </c>
@@ -13971,7 +13970,7 @@
       <c r="AX160" s="10"/>
       <c r="AY160" s="10"/>
     </row>
-    <row r="161" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>58792</v>
       </c>
@@ -14060,7 +14059,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="162" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>54909</v>
       </c>
@@ -14147,7 +14146,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>61405</v>
       </c>
@@ -14218,7 +14217,7 @@
       <c r="AX163" s="10"/>
       <c r="AY163" s="10"/>
     </row>
-    <row r="164" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>59973</v>
       </c>
@@ -14289,7 +14288,7 @@
       <c r="AX164" s="10"/>
       <c r="AY164" s="10"/>
     </row>
-    <row r="165" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>60626</v>
       </c>
@@ -14360,7 +14359,7 @@
       <c r="AX165" s="10"/>
       <c r="AY165" s="10"/>
     </row>
-    <row r="166" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>64877</v>
       </c>
@@ -14431,7 +14430,7 @@
       <c r="AX166" s="10"/>
       <c r="AY166" s="10"/>
     </row>
-    <row r="167" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>64911</v>
       </c>
@@ -14502,7 +14501,7 @@
       <c r="AX167" s="10"/>
       <c r="AY167" s="10"/>
     </row>
-    <row r="168" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>62802</v>
       </c>
@@ -14573,7 +14572,7 @@
       <c r="AX168" s="10"/>
       <c r="AY168" s="10"/>
     </row>
-    <row r="169" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>62261</v>
       </c>
@@ -14644,7 +14643,7 @@
       <c r="AX169" s="10"/>
       <c r="AY169" s="10"/>
     </row>
-    <row r="170" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>61704</v>
       </c>
@@ -14721,7 +14720,7 @@
       </c>
       <c r="AY170" s="10"/>
     </row>
-    <row r="171" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>61409</v>
       </c>
@@ -14792,7 +14791,7 @@
       <c r="AX171" s="10"/>
       <c r="AY171" s="10"/>
     </row>
-    <row r="172" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>64883</v>
       </c>
@@ -14863,7 +14862,7 @@
       <c r="AX172" s="10"/>
       <c r="AY172" s="10"/>
     </row>
-    <row r="173" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>63631</v>
       </c>
@@ -14952,7 +14951,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="174" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>66104</v>
       </c>
@@ -15041,7 +15040,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="175" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>65700</v>
       </c>
@@ -15112,7 +15111,7 @@
       <c r="AX175" s="10"/>
       <c r="AY175" s="10"/>
     </row>
-    <row r="176" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>65702</v>
       </c>
@@ -15183,7 +15182,7 @@
       <c r="AX176" s="10"/>
       <c r="AY176" s="10"/>
     </row>
-    <row r="177" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>63650</v>
       </c>
@@ -15274,7 +15273,7 @@
       <c r="AX177" s="10"/>
       <c r="AY177" s="10"/>
     </row>
-    <row r="178" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>64147</v>
       </c>
@@ -15345,7 +15344,7 @@
       <c r="AX178" s="10"/>
       <c r="AY178" s="10"/>
     </row>
-    <row r="179" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>68627</v>
       </c>
@@ -15416,7 +15415,7 @@
       <c r="AX179" s="10"/>
       <c r="AY179" s="10"/>
     </row>
-    <row r="180" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>69182</v>
       </c>
@@ -15487,7 +15486,7 @@
       <c r="AX180" s="10"/>
       <c r="AY180" s="10"/>
     </row>
-    <row r="181" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>68620</v>
       </c>
@@ -15558,7 +15557,7 @@
       <c r="AX181" s="10"/>
       <c r="AY181" s="10"/>
     </row>
-    <row r="182" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>67311</v>
       </c>
@@ -15629,7 +15628,7 @@
       <c r="AX182" s="10"/>
       <c r="AY182" s="10"/>
     </row>
-    <row r="183" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>68293</v>
       </c>
@@ -15700,7 +15699,7 @@
       <c r="AX183" s="10"/>
       <c r="AY183" s="10"/>
     </row>
-    <row r="184" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>67733</v>
       </c>
@@ -15771,7 +15770,7 @@
       <c r="AX184" s="10"/>
       <c r="AY184" s="10"/>
     </row>
-    <row r="185" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>67978</v>
       </c>
@@ -15842,7 +15841,7 @@
       <c r="AX185" s="10"/>
       <c r="AY185" s="10"/>
     </row>
-    <row r="186" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>70400</v>
       </c>
@@ -15913,7 +15912,7 @@
       <c r="AX186" s="10"/>
       <c r="AY186" s="10"/>
     </row>
-    <row r="187" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>70040</v>
       </c>
@@ -15984,7 +15983,7 @@
       <c r="AX187" s="10"/>
       <c r="AY187" s="10"/>
     </row>
-    <row r="188" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>69319</v>
       </c>
@@ -16055,7 +16054,7 @@
       <c r="AX188" s="10"/>
       <c r="AY188" s="10"/>
     </row>
-    <row r="189" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>70602</v>
       </c>
@@ -16126,7 +16125,7 @@
       <c r="AX189" s="10"/>
       <c r="AY189" s="10"/>
     </row>
-    <row r="190" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>71241</v>
       </c>
@@ -16215,7 +16214,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="191" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>69732</v>
       </c>
@@ -16304,7 +16303,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="192" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>72560</v>
       </c>
@@ -16375,7 +16374,7 @@
       <c r="AX192" s="10"/>
       <c r="AY192" s="10"/>
     </row>
-    <row r="193" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>74212</v>
       </c>
@@ -16470,7 +16469,7 @@
       </c>
       <c r="AY193" s="10"/>
     </row>
-    <row r="194" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>71440</v>
       </c>
@@ -16557,7 +16556,7 @@
       <c r="AX194" s="10"/>
       <c r="AY194" s="10"/>
     </row>
-    <row r="195" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>71592</v>
       </c>
@@ -16628,7 +16627,7 @@
       <c r="AX195" s="10"/>
       <c r="AY195" s="10"/>
     </row>
-    <row r="196" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>73881</v>
       </c>
@@ -16713,7 +16712,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="197" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>73949</v>
       </c>
@@ -16794,7 +16793,7 @@
       <c r="AX197" s="10"/>
       <c r="AY197" s="10"/>
     </row>
-    <row r="198" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>72507</v>
       </c>
@@ -16865,7 +16864,7 @@
       <c r="AX198" s="10"/>
       <c r="AY198" s="10"/>
     </row>
-    <row r="199" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>71904</v>
       </c>
@@ -16936,7 +16935,7 @@
       <c r="AX199" s="10"/>
       <c r="AY199" s="10"/>
     </row>
-    <row r="200" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>73226</v>
       </c>
@@ -17007,7 +17006,7 @@
       <c r="AX200" s="10"/>
       <c r="AY200" s="10"/>
     </row>
-    <row r="201" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>72184</v>
       </c>
@@ -17078,7 +17077,7 @@
       <c r="AX201" s="10"/>
       <c r="AY201" s="10"/>
     </row>
-    <row r="202" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>73518</v>
       </c>
@@ -17149,7 +17148,7 @@
       <c r="AX202" s="10"/>
       <c r="AY202" s="10"/>
     </row>
-    <row r="203" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>73453</v>
       </c>
@@ -17220,7 +17219,7 @@
       <c r="AX203" s="10"/>
       <c r="AY203" s="10"/>
     </row>
-    <row r="204" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>74766</v>
       </c>
@@ -17291,7 +17290,7 @@
       <c r="AX204" s="10"/>
       <c r="AY204" s="10"/>
     </row>
-    <row r="205" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>75496</v>
       </c>
@@ -17378,7 +17377,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="206" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>2402</v>
       </c>
@@ -17449,7 +17448,7 @@
       <c r="AX206" s="10"/>
       <c r="AY206" s="10"/>
     </row>
-    <row r="207" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>19502</v>
       </c>
@@ -17520,7 +17519,7 @@
       <c r="AX207" s="10"/>
       <c r="AY207" s="10"/>
     </row>
-    <row r="208" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>26368</v>
       </c>
@@ -17591,7 +17590,7 @@
       <c r="AX208" s="10"/>
       <c r="AY208" s="10"/>
     </row>
-    <row r="209" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>26584</v>
       </c>
@@ -17662,7 +17661,7 @@
       <c r="AX209" s="10"/>
       <c r="AY209" s="10"/>
     </row>
-    <row r="210" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>27235</v>
       </c>
@@ -17733,7 +17732,7 @@
       <c r="AX210" s="10"/>
       <c r="AY210" s="10"/>
     </row>
-    <row r="211" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>32587</v>
       </c>
@@ -17804,7 +17803,7 @@
       <c r="AX211" s="10"/>
       <c r="AY211" s="10"/>
     </row>
-    <row r="212" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>35666</v>
       </c>
@@ -17875,7 +17874,7 @@
       <c r="AX212" s="10"/>
       <c r="AY212" s="10"/>
     </row>
-    <row r="213" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>38951</v>
       </c>
@@ -17946,7 +17945,7 @@
       <c r="AX213" s="10"/>
       <c r="AY213" s="10"/>
     </row>
-    <row r="214" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>50001</v>
       </c>
@@ -18017,7 +18016,7 @@
       <c r="AX214" s="10"/>
       <c r="AY214" s="10"/>
     </row>
-    <row r="215" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>53883</v>
       </c>
@@ -18088,7 +18087,7 @@
       <c r="AX215" s="10"/>
       <c r="AY215" s="10"/>
     </row>
-    <row r="216" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>73454</v>
       </c>
@@ -18159,7 +18158,7 @@
       <c r="AX216" s="10"/>
       <c r="AY216" s="10"/>
     </row>
-    <row r="217" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>84560</v>
       </c>
@@ -18230,7 +18229,7 @@
       <c r="AX217" s="10"/>
       <c r="AY217" s="10"/>
     </row>
-    <row r="218" spans="1:51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>84924</v>
       </c>
@@ -18301,7 +18300,7 @@
       <c r="AX218" s="10"/>
       <c r="AY218" s="10"/>
     </row>
-    <row r="219" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>84233</v>
       </c>
@@ -18390,7 +18389,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="220" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>79434</v>
       </c>
@@ -18461,7 +18460,7 @@
       <c r="AX220" s="10"/>
       <c r="AY220" s="10"/>
     </row>
-    <row r="221" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>77854</v>
       </c>
@@ -18532,7 +18531,7 @@
       <c r="AX221" s="10"/>
       <c r="AY221" s="10"/>
     </row>
-    <row r="222" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>74215</v>
       </c>
@@ -18603,7 +18602,7 @@
       <c r="AX222" s="10"/>
       <c r="AY222" s="10"/>
     </row>
-    <row r="223" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>77572</v>
       </c>
@@ -18674,7 +18673,7 @@
       <c r="AX223" s="10"/>
       <c r="AY223" s="10"/>
     </row>
-    <row r="224" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>77545</v>
       </c>
@@ -18745,7 +18744,7 @@
       <c r="AX224" s="10"/>
       <c r="AY224" s="10"/>
     </row>
-    <row r="225" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>74516</v>
       </c>
@@ -18816,7 +18815,7 @@
       <c r="AX225" s="10"/>
       <c r="AY225" s="10"/>
     </row>
-    <row r="226" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>77481</v>
       </c>
@@ -18903,7 +18902,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="227" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>77520</v>
       </c>
@@ -18990,7 +18989,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="228" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>76914</v>
       </c>
@@ -19067,7 +19066,7 @@
       <c r="AX228" s="10"/>
       <c r="AY228" s="10"/>
     </row>
-    <row r="229" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>77534</v>
       </c>
@@ -19154,7 +19153,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="230" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>79433</v>
       </c>
@@ -19245,7 +19244,7 @@
       <c r="AX230" s="10"/>
       <c r="AY230" s="10"/>
     </row>
-    <row r="231" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <v>79922</v>
       </c>
@@ -19316,7 +19315,7 @@
       <c r="AX231" s="10"/>
       <c r="AY231" s="10"/>
     </row>
-    <row r="232" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <v>82708</v>
       </c>
@@ -19387,7 +19386,7 @@
       <c r="AX232" s="10"/>
       <c r="AY232" s="10"/>
     </row>
-    <row r="233" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
         <v>82991</v>
       </c>
@@ -19458,7 +19457,7 @@
       <c r="AX233" s="10"/>
       <c r="AY233" s="10"/>
     </row>
-    <row r="234" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <v>82534</v>
       </c>
@@ -19529,7 +19528,7 @@
       <c r="AX234" s="10"/>
       <c r="AY234" s="10"/>
     </row>
-    <row r="235" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
         <v>81260</v>
       </c>
@@ -19618,7 +19617,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="236" spans="1:51" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:51" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
         <v>82651</v>
       </c>
@@ -19705,7 +19704,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="237" spans="1:51" ht="52.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:51" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <v>83738</v>
       </c>
@@ -19778,7 +19777,7 @@
       <c r="AX237" s="10"/>
       <c r="AY237" s="10"/>
     </row>
-    <row r="238" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
         <v>82651</v>
       </c>
@@ -19849,7 +19848,7 @@
       <c r="AX238" s="10"/>
       <c r="AY238" s="10"/>
     </row>
-    <row r="239" spans="1:51" ht="23.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <v>82710</v>
       </c>
@@ -19920,7 +19919,7 @@
       <c r="AX239" s="10"/>
       <c r="AY239" s="10"/>
     </row>
-    <row r="240" spans="1:51" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:51" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
         <v>83688</v>
       </c>
@@ -20020,19 +20019,19 @@
     <row r="243" spans="7:52" x14ac:dyDescent="0.25">
       <c r="K243">
         <f>SUBTOTAL(103,K$2:K$240)</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="L243">
         <f t="shared" ref="L243:AY243" si="0">SUBTOTAL(103,L$2:L$240)</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="M243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="N243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O243">
         <f t="shared" si="0"/>
@@ -20040,7 +20039,7 @@
       </c>
       <c r="P243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q243">
         <f t="shared" si="0"/>
@@ -20048,15 +20047,15 @@
       </c>
       <c r="R243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="S243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="T243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="U243">
         <f t="shared" si="0"/>
@@ -20064,19 +20063,19 @@
       </c>
       <c r="V243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="W243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="Y243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="Z243">
         <f t="shared" si="0"/>
@@ -20088,11 +20087,11 @@
       </c>
       <c r="AB243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AD243">
         <f t="shared" si="0"/>
@@ -20108,7 +20107,7 @@
       </c>
       <c r="AG243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="AH243">
         <f t="shared" si="0"/>
@@ -20116,19 +20115,19 @@
       </c>
       <c r="AI243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AJ243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AK243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="AL243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="AM243">
         <f t="shared" si="0"/>
@@ -20144,15 +20143,15 @@
       </c>
       <c r="AP243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AQ243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="AR243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="AS243">
         <f t="shared" si="0"/>
@@ -20160,11 +20159,11 @@
       </c>
       <c r="AT243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="AU243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AV243">
         <f t="shared" si="0"/>
@@ -20176,77 +20175,77 @@
       </c>
       <c r="AX243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="AY243">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="AZ243">
         <f>SUM(K243:AY243)</f>
-        <v>0</v>
+        <v>962</v>
       </c>
     </row>
     <row r="244" spans="7:52" x14ac:dyDescent="0.25">
-      <c r="K244" t="str">
+      <c r="K244">
         <f>IFERROR(SUBTOTAL(101,K$2:K$240),"")</f>
-        <v/>
-      </c>
-      <c r="L244" t="str">
+        <v>89.583333333333329</v>
+      </c>
+      <c r="L244">
         <f t="shared" ref="L244:AY244" si="1">IFERROR(SUBTOTAL(101,L$2:L$240),"")</f>
-        <v/>
-      </c>
-      <c r="M244" t="str">
+        <v>54.729729729729726</v>
+      </c>
+      <c r="M244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N244" t="str">
+        <v>11.824324324324325</v>
+      </c>
+      <c r="N244">
         <f t="shared" si="1"/>
-        <v/>
+        <v>58.59375</v>
       </c>
       <c r="O244" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P244" t="str">
+      <c r="P244">
         <f t="shared" si="1"/>
-        <v/>
+        <v>90.625</v>
       </c>
       <c r="Q244" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="R244" t="str">
+      <c r="R244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="S244" t="str">
+        <v>74.431818181818187</v>
+      </c>
+      <c r="S244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="T244" t="str">
+        <v>3.4090909090909092</v>
+      </c>
+      <c r="T244">
         <f t="shared" si="1"/>
-        <v/>
+        <v>55.921052631578945</v>
       </c>
       <c r="U244" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="V244" t="str">
+      <c r="V244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="W244" t="str">
+        <v>40.517241379310342</v>
+      </c>
+      <c r="W244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X244" t="str">
+        <v>0</v>
+      </c>
+      <c r="X244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Y244" t="str">
+        <v>73.529411764705884</v>
+      </c>
+      <c r="Y244">
         <f t="shared" si="1"/>
-        <v/>
+        <v>55.263157894736842</v>
       </c>
       <c r="Z244" t="str">
         <f t="shared" si="1"/>
@@ -20256,13 +20255,13 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AB244" t="str">
+      <c r="AB244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AC244" t="str">
+        <v>0</v>
+      </c>
+      <c r="AC244">
         <f t="shared" si="1"/>
-        <v/>
+        <v>25</v>
       </c>
       <c r="AD244" t="str">
         <f t="shared" si="1"/>
@@ -20276,29 +20275,29 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AG244" t="str">
+      <c r="AG244">
         <f t="shared" si="1"/>
-        <v/>
+        <v>46.276595744680854</v>
       </c>
       <c r="AH244" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AI244" t="str">
+      <c r="AI244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AJ244" t="str">
+        <v>71.25</v>
+      </c>
+      <c r="AJ244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AK244" t="str">
+        <v>37.068965517241381</v>
+      </c>
+      <c r="AK244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AL244" t="str">
+        <v>94.811320754716988</v>
+      </c>
+      <c r="AL244">
         <f t="shared" si="1"/>
-        <v/>
+        <v>80.232558139534888</v>
       </c>
       <c r="AM244" t="str">
         <f t="shared" si="1"/>
@@ -20312,29 +20311,29 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AP244" t="str">
+      <c r="AP244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AQ244" t="str">
+        <v>75</v>
+      </c>
+      <c r="AQ244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AR244" t="str">
+        <v>30.434782608695652</v>
+      </c>
+      <c r="AR244">
         <f t="shared" si="1"/>
-        <v/>
+        <v>82.38636363636364</v>
       </c>
       <c r="AS244" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AT244" t="str">
+      <c r="AT244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AU244" t="str">
+        <v>82.608695652173907</v>
+      </c>
+      <c r="AU244">
         <f t="shared" si="1"/>
-        <v/>
+        <v>50</v>
       </c>
       <c r="AV244" t="str">
         <f t="shared" si="1"/>
@@ -20344,21 +20343,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AX244" t="str">
+      <c r="AX244">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AY244" t="str">
+        <v>60.439560439560438</v>
+      </c>
+      <c r="AY244">
         <f t="shared" si="1"/>
-        <v/>
+        <v>96.296296296296291</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AY242" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AY242" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -20371,7 +20366,7 @@
   <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A42"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -20379,31 +20374,31 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>Sheet1!AZ243</f>
-        <v>0</v>
+        <v>962</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
+      <c r="A2">
         <f>Sheet1!K244</f>
-        <v/>
+        <v>89.583333333333329</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
+      <c r="A3">
         <f>Sheet1!L244</f>
-        <v/>
+        <v>54.729729729729726</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
+      <c r="A4">
         <f>Sheet1!M244</f>
-        <v/>
+        <v>11.824324324324325</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
+      <c r="A5">
         <f>Sheet1!N244</f>
-        <v/>
+        <v>58.59375</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -20413,9 +20408,9 @@
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
+      <c r="A7">
         <f>Sheet1!P244</f>
-        <v/>
+        <v>90.625</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -20425,21 +20420,21 @@
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
+      <c r="A9">
         <f>Sheet1!R244</f>
-        <v/>
+        <v>74.431818181818187</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
+      <c r="A10">
         <f>Sheet1!S244</f>
-        <v/>
+        <v>3.4090909090909092</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
+      <c r="A11">
         <f>Sheet1!T244</f>
-        <v/>
+        <v>55.921052631578945</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -20449,27 +20444,27 @@
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
+      <c r="A13">
         <f>Sheet1!V244</f>
-        <v/>
+        <v>40.517241379310342</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
+      <c r="A14">
         <f>Sheet1!W244</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
+      <c r="A15">
         <f>Sheet1!X244</f>
-        <v/>
+        <v>73.529411764705884</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="str">
+      <c r="A16">
         <f>Sheet1!Y244</f>
-        <v/>
+        <v>55.263157894736842</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -20485,15 +20480,15 @@
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
+      <c r="A19">
         <f>Sheet1!AB244</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="str">
+      <c r="A20">
         <f>Sheet1!AC244</f>
-        <v/>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -20515,9 +20510,9 @@
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
+      <c r="A24">
         <f>Sheet1!AG244</f>
-        <v/>
+        <v>46.276595744680854</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
@@ -20527,27 +20522,27 @@
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
+      <c r="A26">
         <f>Sheet1!AI244</f>
-        <v/>
+        <v>71.25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
+      <c r="A27">
         <f>Sheet1!AJ244</f>
-        <v/>
+        <v>37.068965517241381</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
+      <c r="A28">
         <f>Sheet1!AK244</f>
-        <v/>
+        <v>94.811320754716988</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="str">
+      <c r="A29">
         <f>Sheet1!AL244</f>
-        <v/>
+        <v>80.232558139534888</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -20569,21 +20564,21 @@
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="str">
+      <c r="A33">
         <f>Sheet1!AP244</f>
-        <v/>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="str">
+      <c r="A34">
         <f>Sheet1!AQ244</f>
-        <v/>
+        <v>30.434782608695652</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="str">
+      <c r="A35">
         <f>Sheet1!AR244</f>
-        <v/>
+        <v>82.38636363636364</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -20593,15 +20588,15 @@
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="str">
+      <c r="A37">
         <f>Sheet1!AT244</f>
-        <v/>
+        <v>82.608695652173907</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="str">
+      <c r="A38">
         <f>Sheet1!AU244</f>
-        <v/>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
@@ -20617,15 +20612,15 @@
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="str">
+      <c r="A41">
         <f>Sheet1!AX244</f>
-        <v/>
+        <v>60.439560439560438</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="str">
+      <c r="A42">
         <f>Sheet1!AY244</f>
-        <v/>
+        <v>96.296296296296291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>